<commit_message>
Web Office - Initial Stuff, Searching on trade/name/Phone from WO Search Header - Progressing
</commit_message>
<xml_diff>
--- a/Data Files/Search_Data.xlsx
+++ b/Data Files/Search_Data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\davidho\Katalon Studio\Start\Data Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5362AED-D205-40B9-8528-3F3CC61CA04B}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83BCDD60-9DF5-4890-B151-A0623518EBAB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4845" yWindow="6045" windowWidth="21600" windowHeight="7020" xr2:uid="{56648964-8086-4401-B8BD-AFCFF037A6DE}"/>
+    <workbookView minimized="1" xWindow="4035" yWindow="2415" windowWidth="21600" windowHeight="11385" xr2:uid="{56648964-8086-4401-B8BD-AFCFF037A6DE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="63">
   <si>
     <t>Tree Surgeon</t>
   </si>
@@ -169,16 +169,94 @@
   </si>
   <si>
     <t>Blocked Sinks in Rugby</t>
+  </si>
+  <si>
+    <t>address</t>
+  </si>
+  <si>
+    <t>70 Worthing Avenue, Gosport, Hampshire, PO12 4DH</t>
+  </si>
+  <si>
+    <t>023 9258 3018</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>fostertreecare@tiscali.co.uk</t>
+  </si>
+  <si>
+    <t>mobile</t>
+  </si>
+  <si>
+    <t>07818 446596</t>
+  </si>
+  <si>
+    <t>join_Date</t>
+  </si>
+  <si>
+    <t>dob</t>
+  </si>
+  <si>
+    <t>website</t>
+  </si>
+  <si>
+    <t>checkatrade.com/FosterTreeCare</t>
+  </si>
+  <si>
+    <t>24 Burney Road, Gosport, Hampshire, PO12 2QB</t>
+  </si>
+  <si>
+    <t>07787 612040</t>
+  </si>
+  <si>
+    <t>skyfelltrees@gmail.com</t>
+  </si>
+  <si>
+    <t>contact</t>
+  </si>
+  <si>
+    <t>07787 620324</t>
+  </si>
+  <si>
+    <t>checkatrade.com/SkyfellTreeSpecialists</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF555555"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF555555"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF262626"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -201,10 +279,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -212,8 +291,21 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -526,10 +618,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84D56B88-33E9-468B-853E-05EE5D8A6600}">
-  <dimension ref="A1:J6"/>
+  <dimension ref="A1:Q6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="L1" sqref="L1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -540,13 +632,19 @@
     <col min="4" max="4" width="17" customWidth="1"/>
     <col min="5" max="5" width="20.5703125" customWidth="1"/>
     <col min="6" max="6" width="15.140625" customWidth="1"/>
-    <col min="7" max="7" width="47.140625" customWidth="1"/>
-    <col min="8" max="8" width="53.5703125" customWidth="1"/>
-    <col min="9" max="9" width="18.7109375" customWidth="1"/>
-    <col min="10" max="10" width="13.5703125" customWidth="1"/>
+    <col min="7" max="7" width="36.28515625" customWidth="1"/>
+    <col min="8" max="8" width="28.85546875" customWidth="1"/>
+    <col min="9" max="9" width="15.28515625" customWidth="1"/>
+    <col min="10" max="10" width="15.85546875" customWidth="1"/>
+    <col min="11" max="11" width="25.5703125" customWidth="1"/>
+    <col min="12" max="13" width="13.7109375" customWidth="1"/>
+    <col min="14" max="14" width="24.5703125" customWidth="1"/>
+    <col min="15" max="15" width="53.5703125" customWidth="1"/>
+    <col min="16" max="16" width="18.7109375" customWidth="1"/>
+    <col min="17" max="17" width="13.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>14</v>
       </c>
@@ -569,16 +667,37 @@
         <v>6</v>
       </c>
       <c r="H1" t="s">
+        <v>46</v>
+      </c>
+      <c r="I1" t="s">
+        <v>51</v>
+      </c>
+      <c r="J1" t="s">
+        <v>60</v>
+      </c>
+      <c r="K1" t="s">
+        <v>49</v>
+      </c>
+      <c r="L1" t="s">
+        <v>53</v>
+      </c>
+      <c r="M1" t="s">
+        <v>54</v>
+      </c>
+      <c r="N1" t="s">
+        <v>55</v>
+      </c>
+      <c r="O1" t="s">
         <v>21</v>
       </c>
-      <c r="I1" t="s">
+      <c r="P1" t="s">
         <v>39</v>
       </c>
-      <c r="J1" t="s">
+      <c r="Q1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>15</v>
       </c>
@@ -600,17 +719,38 @@
       <c r="G2" t="s">
         <v>3</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H2" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="L2" s="6">
+        <v>40721</v>
+      </c>
+      <c r="M2" s="7">
+        <v>27790</v>
+      </c>
+      <c r="N2" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="O2" t="s">
         <v>24</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="P2" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="Q2" s="2" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>16</v>
       </c>
@@ -632,17 +772,38 @@
       <c r="G3" t="s">
         <v>43</v>
       </c>
-      <c r="H3" t="s">
+      <c r="H3" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="J3" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="K3" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="L3" s="6">
+        <v>41739</v>
+      </c>
+      <c r="M3" s="7">
+        <v>29190</v>
+      </c>
+      <c r="N3" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="O3" t="s">
         <v>27</v>
       </c>
-      <c r="I3" s="2">
+      <c r="P3" s="2">
         <v>400</v>
       </c>
-      <c r="J3" s="2">
+      <c r="Q3" s="2">
         <v>600</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>17</v>
       </c>
@@ -664,17 +825,17 @@
       <c r="G4" t="s">
         <v>44</v>
       </c>
-      <c r="H4" t="s">
+      <c r="O4" t="s">
         <v>30</v>
       </c>
-      <c r="I4" s="2">
+      <c r="P4" s="2">
         <v>500</v>
       </c>
-      <c r="J4" s="2">
+      <c r="Q4" s="2">
         <v>700</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>31</v>
       </c>
@@ -696,17 +857,17 @@
       <c r="G5" t="s">
         <v>45</v>
       </c>
-      <c r="H5" t="s">
+      <c r="O5" t="s">
         <v>34</v>
       </c>
-      <c r="I5" s="2">
+      <c r="P5" s="2">
         <v>600</v>
       </c>
-      <c r="J5" s="2">
+      <c r="Q5" s="2">
         <v>800</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>35</v>
       </c>
@@ -728,18 +889,22 @@
       <c r="G6" t="s">
         <v>13</v>
       </c>
-      <c r="H6" t="s">
+      <c r="O6" t="s">
         <v>24</v>
       </c>
-      <c r="I6" s="2">
+      <c r="P6" s="2">
         <v>700</v>
       </c>
-      <c r="J6" s="2">
+      <c r="Q6" s="2">
         <v>900</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="N2" r:id="rId1" display="http://www.checkatrade.com/FosterTreeCare/" xr:uid="{03B599EA-752F-4757-B538-19EF5479C027}"/>
+    <hyperlink ref="N3" r:id="rId2" display="http://www.checkatrade.com/SkyfellTreeSpecialists/" xr:uid="{D97B2C45-4581-498B-A8E1-EA37F0DB8FDD}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added 11 Web Office Tests - Settings->Web Office Area
</commit_message>
<xml_diff>
--- a/Data Files/Search_Data.xlsx
+++ b/Data Files/Search_Data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\davidho\git\src\Data Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11457069-4E16-4FF0-AE09-153CDF0098A2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6F970A1-FFE7-4A04-BEE1-AA397BE0E7A6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{56648964-8086-4401-B8BD-AFCFF037A6DE}"/>
+    <workbookView xWindow="40920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{56648964-8086-4401-B8BD-AFCFF037A6DE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -300,13 +300,13 @@
     <t>Garage/Vehicle Services</t>
   </si>
   <si>
-    <t>Holyhead</t>
-  </si>
-  <si>
     <t>Shrewsbury</t>
   </si>
   <si>
     <t>Rustington</t>
+  </si>
+  <si>
+    <t>Hayling Island</t>
   </si>
 </sst>
 </file>
@@ -746,31 +746,31 @@
   <dimension ref="A1:S6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="2" width="26.28515625" customWidth="1"/>
-    <col min="3" max="3" width="26.42578125" customWidth="1"/>
-    <col min="4" max="4" width="19.42578125" customWidth="1"/>
-    <col min="5" max="5" width="30.5703125" customWidth="1"/>
+    <col min="1" max="2" width="26.265625" customWidth="1"/>
+    <col min="3" max="3" width="26.3984375" customWidth="1"/>
+    <col min="4" max="4" width="19.3984375" customWidth="1"/>
+    <col min="5" max="5" width="30.59765625" customWidth="1"/>
     <col min="6" max="6" width="17" customWidth="1"/>
-    <col min="7" max="7" width="36.42578125" customWidth="1"/>
-    <col min="8" max="8" width="15.140625" customWidth="1"/>
-    <col min="9" max="9" width="36.28515625" customWidth="1"/>
-    <col min="10" max="10" width="28.85546875" customWidth="1"/>
-    <col min="11" max="11" width="15.28515625" customWidth="1"/>
-    <col min="12" max="12" width="15.85546875" customWidth="1"/>
-    <col min="13" max="13" width="25.5703125" customWidth="1"/>
-    <col min="14" max="15" width="13.7109375" customWidth="1"/>
-    <col min="16" max="16" width="35.140625" customWidth="1"/>
-    <col min="17" max="17" width="53.5703125" customWidth="1"/>
-    <col min="18" max="18" width="18.7109375" customWidth="1"/>
-    <col min="19" max="19" width="13.5703125" customWidth="1"/>
+    <col min="7" max="7" width="36.3984375" customWidth="1"/>
+    <col min="8" max="8" width="15.1328125" customWidth="1"/>
+    <col min="9" max="9" width="36.265625" customWidth="1"/>
+    <col min="10" max="10" width="28.86328125" customWidth="1"/>
+    <col min="11" max="11" width="15.265625" customWidth="1"/>
+    <col min="12" max="12" width="15.86328125" customWidth="1"/>
+    <col min="13" max="13" width="25.59765625" customWidth="1"/>
+    <col min="14" max="15" width="13.73046875" customWidth="1"/>
+    <col min="16" max="16" width="35.1328125" customWidth="1"/>
+    <col min="17" max="17" width="53.59765625" customWidth="1"/>
+    <col min="18" max="18" width="18.73046875" customWidth="1"/>
+    <col min="19" max="19" width="13.59765625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>51</v>
       </c>
@@ -829,7 +829,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A2" s="4" t="s">
         <v>45</v>
       </c>
@@ -888,7 +888,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A3" s="8" t="s">
         <v>23</v>
       </c>
@@ -947,7 +947,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>14</v>
       </c>
@@ -958,7 +958,7 @@
         <v>14</v>
       </c>
       <c r="D4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E4" t="s">
         <v>25</v>
@@ -970,7 +970,7 @@
         <v>6</v>
       </c>
       <c r="H4" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="I4" t="s">
         <v>38</v>
@@ -1006,7 +1006,7 @@
         <v>700</v>
       </c>
     </row>
-    <row r="5" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:19" ht="15.4" x14ac:dyDescent="0.45">
       <c r="A5" s="11">
         <v>381198</v>
       </c>
@@ -1062,7 +1062,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="6" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:19" ht="15.4" x14ac:dyDescent="0.45">
       <c r="A6" s="3" t="s">
         <v>75</v>
       </c>
@@ -1085,7 +1085,7 @@
         <v>88</v>
       </c>
       <c r="H6" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="I6" s="14" t="s">
         <v>87</v>

</xml_diff>